<commit_message>
Update mp, hp, exp bar
</commit_message>
<xml_diff>
--- a/Todo&Defect.xlsx
+++ b/Todo&Defect.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
   <si>
     <t>Description</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -182,6 +182,22 @@
   </si>
   <si>
     <t>Fish</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Optimize player jump</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fish</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Solved</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -506,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -715,6 +731,20 @@
         <v>43100</v>
       </c>
     </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="1">
+        <v>43103</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H4"/>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -727,7 +757,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -775,8 +805,17 @@
       <c r="D2" t="s">
         <v>16</v>
       </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
       <c r="F2" s="1">
         <v>43096</v>
+      </c>
+      <c r="G2" s="1">
+        <v>43103</v>
+      </c>
+      <c r="H2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">

</xml_diff>